<commit_message>
Hybrid Automation Framework & Modular Programming
</commit_message>
<xml_diff>
--- a/excel/SauceLabs.xlsx
+++ b/excel/SauceLabs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Valid URL</t>
   </si>
@@ -28,10 +28,31 @@
     <t xml:space="preserve">InValid URL</t>
   </si>
   <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.saucedemo.com/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.saucedemo1.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret_sauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.saucedemo.com/inventory.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghpoiuyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qwertyuiop</t>
   </si>
 </sst>
 </file>
@@ -150,16 +171,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.48"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -169,19 +192,43 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.saucedemo.com/"/>
     <hyperlink ref="B2" r:id="rId2" display="https://www.saucedemo1.com/"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://www.saucedemo.com/inventory.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>